<commit_message>
[IMP] transodoo: reverse charge
</commit_message>
<xml_diff>
--- a/clodoo/transodoo.xlsx
+++ b/clodoo/transodoo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="724">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -1862,9 +1862,6 @@
   </si>
   <si>
     <t xml:space="preserve">l10n_it_reverse_charge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l10n_it_vat_rc_replace</t>
   </si>
   <si>
     <t xml:space="preserve">payment_mode</t>
@@ -2387,10 +2384,10 @@
   </sheetPr>
   <dimension ref="A1:Y445"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="S127" activeCellId="0" sqref="S127"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A352" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A364" activeCellId="0" sqref="A364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7752,7 +7749,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="1" t="s">
         <v>219</v>
       </c>
@@ -7765,9 +7762,7 @@
       <c r="H364" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="V364" s="2" t="s">
-        <v>614</v>
-      </c>
+      <c r="V364" s="2"/>
       <c r="Y364" s="1" t="s">
         <v>199</v>
       </c>
@@ -7813,18 +7808,18 @@
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C368" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F368" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C369" s="1" t="s">
         <v>26</v>
@@ -7835,7 +7830,7 @@
     </row>
     <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C370" s="1" t="s">
         <v>26</v>
@@ -7849,7 +7844,7 @@
     </row>
     <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C371" s="1" t="s">
         <v>26</v>
@@ -7860,7 +7855,7 @@
     </row>
     <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C372" s="1" t="s">
         <v>26</v>
@@ -7874,7 +7869,7 @@
     </row>
     <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C373" s="1" t="s">
         <v>26</v>
@@ -7888,7 +7883,7 @@
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C374" s="1" t="s">
         <v>26</v>
@@ -7899,7 +7894,7 @@
     </row>
     <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C375" s="1" t="s">
         <v>26</v>
@@ -7913,13 +7908,13 @@
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C376" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D376" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F376" s="2" t="s">
         <v>1</v>
@@ -7927,7 +7922,7 @@
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B377" s="2" t="s">
         <v>122</v>
@@ -7936,7 +7931,7 @@
         <v>32</v>
       </c>
       <c r="D377" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G377" s="1" t="s">
         <v>143</v>
@@ -7944,7 +7939,7 @@
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B378" s="2" t="s">
         <v>122</v>
@@ -7953,15 +7948,15 @@
         <v>32</v>
       </c>
       <c r="D378" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="G378" s="1" t="s">
         <v>622</v>
-      </c>
-      <c r="G378" s="1" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B379" s="2" t="s">
         <v>122</v>
@@ -7970,12 +7965,12 @@
         <v>32</v>
       </c>
       <c r="D379" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B380" s="2" t="s">
         <v>122</v>
@@ -7984,15 +7979,15 @@
         <v>32</v>
       </c>
       <c r="D380" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="G380" s="1" t="s">
         <v>625</v>
-      </c>
-      <c r="G380" s="1" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B381" s="2" t="s">
         <v>122</v>
@@ -8001,12 +7996,12 @@
         <v>32</v>
       </c>
       <c r="D381" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B382" s="2" t="s">
         <v>122</v>
@@ -8015,12 +8010,12 @@
         <v>32</v>
       </c>
       <c r="D382" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B383" s="2" t="s">
         <v>122</v>
@@ -8029,7 +8024,7 @@
         <v>32</v>
       </c>
       <c r="D383" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G383" s="1" t="s">
         <v>143</v>
@@ -8037,7 +8032,7 @@
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B384" s="2" t="s">
         <v>122</v>
@@ -8046,7 +8041,7 @@
         <v>32</v>
       </c>
       <c r="D384" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G384" s="1" t="s">
         <v>143</v>
@@ -8054,7 +8049,7 @@
     </row>
     <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B385" s="2" t="s">
         <v>122</v>
@@ -8063,12 +8058,12 @@
         <v>32</v>
       </c>
       <c r="D385" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B386" s="2" t="s">
         <v>122</v>
@@ -8077,12 +8072,12 @@
         <v>32</v>
       </c>
       <c r="D386" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B387" s="2" t="s">
         <v>122</v>
@@ -8091,7 +8086,7 @@
         <v>32</v>
       </c>
       <c r="D387" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G387" s="1" t="s">
         <v>143</v>
@@ -8099,7 +8094,7 @@
     </row>
     <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B388" s="2" t="s">
         <v>122</v>
@@ -8108,7 +8103,7 @@
         <v>32</v>
       </c>
       <c r="D388" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G388" s="1" t="s">
         <v>143</v>
@@ -8116,7 +8111,7 @@
     </row>
     <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B389" s="2" t="s">
         <v>122</v>
@@ -8125,310 +8120,310 @@
         <v>32</v>
       </c>
       <c r="D389" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C390" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D390" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="B391" s="2" t="s">
         <v>634</v>
-      </c>
-      <c r="B391" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="C391" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D391" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B392" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C392" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D392" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="E392" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="E392" s="1" t="s">
+      <c r="G392" s="1" t="s">
         <v>639</v>
-      </c>
-      <c r="G392" s="1" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B393" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C393" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D393" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="E393" s="1" t="s">
         <v>642</v>
-      </c>
-      <c r="E393" s="1" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C394" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D394" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="G394" s="1" t="s">
         <v>645</v>
-      </c>
-      <c r="G394" s="1" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B395" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C395" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D395" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C396" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D396" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="F396" s="2" t="s">
         <v>649</v>
-      </c>
-      <c r="F396" s="2" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B397" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C397" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D397" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="F397" s="2" t="s">
         <v>652</v>
-      </c>
-      <c r="F397" s="2" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B398" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C398" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D398" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="H398" s="2" t="s">
         <v>655</v>
-      </c>
-      <c r="H398" s="2" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B399" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C399" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D399" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F399" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B400" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C400" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D400" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="E400" s="1" t="s">
         <v>660</v>
-      </c>
-      <c r="E400" s="1" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B401" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C401" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D401" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="E401" s="1" t="s">
         <v>663</v>
-      </c>
-      <c r="E401" s="1" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B402" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C402" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D402" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="E402" s="1" t="s">
         <v>666</v>
-      </c>
-      <c r="E402" s="1" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B403" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C403" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D403" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="G403" s="1" t="s">
         <v>669</v>
-      </c>
-      <c r="G403" s="1" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B404" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C404" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D404" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="E404" s="1" t="s">
         <v>672</v>
-      </c>
-      <c r="E404" s="1" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B405" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C405" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D405" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="E405" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="E405" s="1" t="s">
+      <c r="H405" s="2" t="s">
         <v>676</v>
-      </c>
-      <c r="H405" s="2" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B406" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C406" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D406" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F406" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="H406" s="2" t="s">
         <v>679</v>
-      </c>
-      <c r="H406" s="2" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B407" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C407" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D407" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="E407" s="1" t="s">
         <v>682</v>
-      </c>
-      <c r="E407" s="1" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8439,7 +8434,7 @@
         <v>26</v>
       </c>
       <c r="E408" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8450,10 +8445,10 @@
         <v>26</v>
       </c>
       <c r="D409" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="G409" s="1" t="s">
         <v>685</v>
-      </c>
-      <c r="G409" s="1" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8464,7 +8459,7 @@
         <v>26</v>
       </c>
       <c r="E410" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8475,7 +8470,7 @@
         <v>26</v>
       </c>
       <c r="E411" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8486,7 +8481,7 @@
         <v>26</v>
       </c>
       <c r="E412" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8497,10 +8492,10 @@
         <v>26</v>
       </c>
       <c r="D413" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="G413" s="1" t="s">
         <v>690</v>
-      </c>
-      <c r="G413" s="1" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8511,10 +8506,10 @@
         <v>26</v>
       </c>
       <c r="D414" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="G414" s="1" t="s">
         <v>692</v>
-      </c>
-      <c r="G414" s="1" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8525,7 +8520,7 @@
         <v>26</v>
       </c>
       <c r="E415" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8536,7 +8531,7 @@
         <v>26</v>
       </c>
       <c r="E416" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8547,7 +8542,7 @@
         <v>26</v>
       </c>
       <c r="E417" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8558,10 +8553,10 @@
         <v>26</v>
       </c>
       <c r="D418" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="G418" s="1" t="s">
         <v>697</v>
-      </c>
-      <c r="G418" s="1" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8583,90 +8578,90 @@
         <v>26</v>
       </c>
       <c r="E420" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C421" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D421" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="E421" s="1" t="s">
         <v>701</v>
-      </c>
-      <c r="E421" s="1" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C422" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D422" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="E422" s="1" t="s">
         <v>703</v>
-      </c>
-      <c r="E422" s="1" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C423" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E423" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C424" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E424" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C425" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D425" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="E425" s="1" t="s">
         <v>706</v>
-      </c>
-      <c r="E425" s="1" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C426" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D426" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="G426" s="1" t="s">
         <v>709</v>
-      </c>
-      <c r="G426" s="1" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C427" s="1" t="s">
         <v>26</v>
@@ -8680,7 +8675,7 @@
     </row>
     <row r="428" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B428" s="2" t="s">
         <v>122</v>
@@ -8689,12 +8684,12 @@
         <v>32</v>
       </c>
       <c r="D428" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B429" s="2" t="s">
         <v>122</v>
@@ -8703,12 +8698,12 @@
         <v>32</v>
       </c>
       <c r="D429" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B430" s="2" t="s">
         <v>122</v>
@@ -8717,12 +8712,12 @@
         <v>32</v>
       </c>
       <c r="D430" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B431" s="2" t="s">
         <v>122</v>
@@ -8731,7 +8726,7 @@
         <v>32</v>
       </c>
       <c r="D431" s="2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="G431" s="1" t="s">
         <v>100</v>
@@ -8739,7 +8734,7 @@
     </row>
     <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B432" s="2" t="s">
         <v>122</v>
@@ -8748,7 +8743,7 @@
         <v>32</v>
       </c>
       <c r="D432" s="2" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="G432" s="1" t="s">
         <v>100</v>
@@ -8756,7 +8751,7 @@
     </row>
     <row r="433" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B433" s="2" t="s">
         <v>122</v>
@@ -8765,7 +8760,7 @@
         <v>32</v>
       </c>
       <c r="D433" s="2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="G433" s="1" t="s">
         <v>100</v>
@@ -8773,7 +8768,7 @@
     </row>
     <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B434" s="2" t="s">
         <v>122</v>
@@ -8782,12 +8777,12 @@
         <v>32</v>
       </c>
       <c r="D434" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B435" s="2" t="s">
         <v>122</v>
@@ -8796,7 +8791,7 @@
         <v>32</v>
       </c>
       <c r="D435" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="G435" s="1" t="s">
         <v>100</v>
@@ -8804,7 +8799,7 @@
     </row>
     <row r="436" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B436" s="2" t="s">
         <v>122</v>
@@ -8813,7 +8808,7 @@
         <v>32</v>
       </c>
       <c r="D436" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="G436" s="1" t="s">
         <v>100</v>
@@ -8821,18 +8816,18 @@
     </row>
     <row r="437" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C437" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D437" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B438" s="2" t="s">
         <v>122</v>
@@ -8841,12 +8836,12 @@
         <v>32</v>
       </c>
       <c r="D438" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B439" s="2" t="s">
         <v>122</v>
@@ -8855,7 +8850,7 @@
         <v>32</v>
       </c>
       <c r="D439" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H439" s="2" t="s">
         <v>100</v>
@@ -8863,7 +8858,7 @@
     </row>
     <row r="440" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B440" s="2" t="s">
         <v>122</v>
@@ -8872,12 +8867,12 @@
         <v>32</v>
       </c>
       <c r="D440" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B441" s="2" t="s">
         <v>122</v>
@@ -8886,12 +8881,12 @@
         <v>32</v>
       </c>
       <c r="D441" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B442" s="2" t="s">
         <v>122</v>
@@ -8900,37 +8895,37 @@
         <v>32</v>
       </c>
       <c r="D442" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="H442" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C443" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D443" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C444" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D444" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C445" s="1" t="s">
         <v>26</v>
@@ -8939,7 +8934,7 @@
         <v>501</v>
       </c>
       <c r="G445" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] transodoo with recent powerp module definition
</commit_message>
<xml_diff>
--- a/clodoo/transodoo.xlsx
+++ b/clodoo/transodoo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="724">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -1862,9 +1862,6 @@
   </si>
   <si>
     <t xml:space="preserve">l10n_it_reverse_charge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l10n_it_vat_rc_replace</t>
   </si>
   <si>
     <t xml:space="preserve">payment_mode</t>
@@ -2387,10 +2384,10 @@
   </sheetPr>
   <dimension ref="A1:Y445"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="S127" activeCellId="0" sqref="S127"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A345" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="V364" activeCellId="0" sqref="V364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7752,7 +7749,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="1" t="s">
         <v>219</v>
       </c>
@@ -7765,9 +7762,7 @@
       <c r="H364" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="V364" s="2" t="s">
-        <v>614</v>
-      </c>
+      <c r="V364" s="2"/>
       <c r="Y364" s="1" t="s">
         <v>199</v>
       </c>
@@ -7813,18 +7808,18 @@
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C368" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F368" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C369" s="1" t="s">
         <v>26</v>
@@ -7835,7 +7830,7 @@
     </row>
     <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C370" s="1" t="s">
         <v>26</v>
@@ -7849,7 +7844,7 @@
     </row>
     <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C371" s="1" t="s">
         <v>26</v>
@@ -7860,7 +7855,7 @@
     </row>
     <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C372" s="1" t="s">
         <v>26</v>
@@ -7874,7 +7869,7 @@
     </row>
     <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C373" s="1" t="s">
         <v>26</v>
@@ -7888,7 +7883,7 @@
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C374" s="1" t="s">
         <v>26</v>
@@ -7899,7 +7894,7 @@
     </row>
     <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C375" s="1" t="s">
         <v>26</v>
@@ -7913,13 +7908,13 @@
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C376" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D376" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F376" s="2" t="s">
         <v>1</v>
@@ -7927,7 +7922,7 @@
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B377" s="2" t="s">
         <v>122</v>
@@ -7936,7 +7931,7 @@
         <v>32</v>
       </c>
       <c r="D377" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G377" s="1" t="s">
         <v>143</v>
@@ -7944,7 +7939,7 @@
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B378" s="2" t="s">
         <v>122</v>
@@ -7953,15 +7948,15 @@
         <v>32</v>
       </c>
       <c r="D378" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="G378" s="1" t="s">
         <v>622</v>
-      </c>
-      <c r="G378" s="1" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B379" s="2" t="s">
         <v>122</v>
@@ -7970,12 +7965,12 @@
         <v>32</v>
       </c>
       <c r="D379" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B380" s="2" t="s">
         <v>122</v>
@@ -7984,15 +7979,15 @@
         <v>32</v>
       </c>
       <c r="D380" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="G380" s="1" t="s">
         <v>625</v>
-      </c>
-      <c r="G380" s="1" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B381" s="2" t="s">
         <v>122</v>
@@ -8001,12 +7996,12 @@
         <v>32</v>
       </c>
       <c r="D381" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B382" s="2" t="s">
         <v>122</v>
@@ -8015,12 +8010,12 @@
         <v>32</v>
       </c>
       <c r="D382" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B383" s="2" t="s">
         <v>122</v>
@@ -8029,7 +8024,7 @@
         <v>32</v>
       </c>
       <c r="D383" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G383" s="1" t="s">
         <v>143</v>
@@ -8037,7 +8032,7 @@
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B384" s="2" t="s">
         <v>122</v>
@@ -8046,7 +8041,7 @@
         <v>32</v>
       </c>
       <c r="D384" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G384" s="1" t="s">
         <v>143</v>
@@ -8054,7 +8049,7 @@
     </row>
     <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B385" s="2" t="s">
         <v>122</v>
@@ -8063,12 +8058,12 @@
         <v>32</v>
       </c>
       <c r="D385" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B386" s="2" t="s">
         <v>122</v>
@@ -8077,12 +8072,12 @@
         <v>32</v>
       </c>
       <c r="D386" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B387" s="2" t="s">
         <v>122</v>
@@ -8091,7 +8086,7 @@
         <v>32</v>
       </c>
       <c r="D387" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G387" s="1" t="s">
         <v>143</v>
@@ -8099,7 +8094,7 @@
     </row>
     <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B388" s="2" t="s">
         <v>122</v>
@@ -8108,7 +8103,7 @@
         <v>32</v>
       </c>
       <c r="D388" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G388" s="1" t="s">
         <v>143</v>
@@ -8116,7 +8111,7 @@
     </row>
     <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B389" s="2" t="s">
         <v>122</v>
@@ -8125,310 +8120,310 @@
         <v>32</v>
       </c>
       <c r="D389" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C390" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D390" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="B391" s="2" t="s">
         <v>634</v>
-      </c>
-      <c r="B391" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="C391" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D391" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B392" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C392" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D392" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="E392" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="E392" s="1" t="s">
+      <c r="G392" s="1" t="s">
         <v>639</v>
-      </c>
-      <c r="G392" s="1" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B393" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C393" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D393" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="E393" s="1" t="s">
         <v>642</v>
-      </c>
-      <c r="E393" s="1" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C394" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D394" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="G394" s="1" t="s">
         <v>645</v>
-      </c>
-      <c r="G394" s="1" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B395" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C395" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D395" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C396" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D396" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="F396" s="2" t="s">
         <v>649</v>
-      </c>
-      <c r="F396" s="2" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B397" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C397" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D397" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="F397" s="2" t="s">
         <v>652</v>
-      </c>
-      <c r="F397" s="2" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B398" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C398" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D398" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="H398" s="2" t="s">
         <v>655</v>
-      </c>
-      <c r="H398" s="2" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B399" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C399" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D399" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F399" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B400" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C400" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D400" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="E400" s="1" t="s">
         <v>660</v>
-      </c>
-      <c r="E400" s="1" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B401" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C401" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D401" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="E401" s="1" t="s">
         <v>663</v>
-      </c>
-      <c r="E401" s="1" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B402" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C402" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D402" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="E402" s="1" t="s">
         <v>666</v>
-      </c>
-      <c r="E402" s="1" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B403" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C403" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D403" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="G403" s="1" t="s">
         <v>669</v>
-      </c>
-      <c r="G403" s="1" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B404" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C404" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D404" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="E404" s="1" t="s">
         <v>672</v>
-      </c>
-      <c r="E404" s="1" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B405" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C405" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D405" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="E405" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="E405" s="1" t="s">
+      <c r="H405" s="2" t="s">
         <v>676</v>
-      </c>
-      <c r="H405" s="2" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B406" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C406" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D406" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F406" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="H406" s="2" t="s">
         <v>679</v>
-      </c>
-      <c r="H406" s="2" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B407" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C407" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D407" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="E407" s="1" t="s">
         <v>682</v>
-      </c>
-      <c r="E407" s="1" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8439,7 +8434,7 @@
         <v>26</v>
       </c>
       <c r="E408" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8450,10 +8445,10 @@
         <v>26</v>
       </c>
       <c r="D409" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="G409" s="1" t="s">
         <v>685</v>
-      </c>
-      <c r="G409" s="1" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8464,7 +8459,7 @@
         <v>26</v>
       </c>
       <c r="E410" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8475,7 +8470,7 @@
         <v>26</v>
       </c>
       <c r="E411" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8486,7 +8481,7 @@
         <v>26</v>
       </c>
       <c r="E412" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8497,10 +8492,10 @@
         <v>26</v>
       </c>
       <c r="D413" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="G413" s="1" t="s">
         <v>690</v>
-      </c>
-      <c r="G413" s="1" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8511,10 +8506,10 @@
         <v>26</v>
       </c>
       <c r="D414" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="G414" s="1" t="s">
         <v>692</v>
-      </c>
-      <c r="G414" s="1" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8525,7 +8520,7 @@
         <v>26</v>
       </c>
       <c r="E415" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8536,7 +8531,7 @@
         <v>26</v>
       </c>
       <c r="E416" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8547,7 +8542,7 @@
         <v>26</v>
       </c>
       <c r="E417" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8558,10 +8553,10 @@
         <v>26</v>
       </c>
       <c r="D418" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="G418" s="1" t="s">
         <v>697</v>
-      </c>
-      <c r="G418" s="1" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8583,90 +8578,90 @@
         <v>26</v>
       </c>
       <c r="E420" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C421" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D421" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="E421" s="1" t="s">
         <v>701</v>
-      </c>
-      <c r="E421" s="1" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C422" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D422" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="E422" s="1" t="s">
         <v>703</v>
-      </c>
-      <c r="E422" s="1" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C423" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E423" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C424" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E424" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C425" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D425" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="E425" s="1" t="s">
         <v>706</v>
-      </c>
-      <c r="E425" s="1" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C426" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D426" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="G426" s="1" t="s">
         <v>709</v>
-      </c>
-      <c r="G426" s="1" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C427" s="1" t="s">
         <v>26</v>
@@ -8680,7 +8675,7 @@
     </row>
     <row r="428" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B428" s="2" t="s">
         <v>122</v>
@@ -8689,12 +8684,12 @@
         <v>32</v>
       </c>
       <c r="D428" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B429" s="2" t="s">
         <v>122</v>
@@ -8703,12 +8698,12 @@
         <v>32</v>
       </c>
       <c r="D429" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B430" s="2" t="s">
         <v>122</v>
@@ -8717,12 +8712,12 @@
         <v>32</v>
       </c>
       <c r="D430" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B431" s="2" t="s">
         <v>122</v>
@@ -8731,7 +8726,7 @@
         <v>32</v>
       </c>
       <c r="D431" s="2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="G431" s="1" t="s">
         <v>100</v>
@@ -8739,7 +8734,7 @@
     </row>
     <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B432" s="2" t="s">
         <v>122</v>
@@ -8748,7 +8743,7 @@
         <v>32</v>
       </c>
       <c r="D432" s="2" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="G432" s="1" t="s">
         <v>100</v>
@@ -8756,7 +8751,7 @@
     </row>
     <row r="433" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B433" s="2" t="s">
         <v>122</v>
@@ -8765,7 +8760,7 @@
         <v>32</v>
       </c>
       <c r="D433" s="2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="G433" s="1" t="s">
         <v>100</v>
@@ -8773,7 +8768,7 @@
     </row>
     <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B434" s="2" t="s">
         <v>122</v>
@@ -8782,12 +8777,12 @@
         <v>32</v>
       </c>
       <c r="D434" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B435" s="2" t="s">
         <v>122</v>
@@ -8796,7 +8791,7 @@
         <v>32</v>
       </c>
       <c r="D435" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="G435" s="1" t="s">
         <v>100</v>
@@ -8804,7 +8799,7 @@
     </row>
     <row r="436" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B436" s="2" t="s">
         <v>122</v>
@@ -8813,7 +8808,7 @@
         <v>32</v>
       </c>
       <c r="D436" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="G436" s="1" t="s">
         <v>100</v>
@@ -8821,18 +8816,18 @@
     </row>
     <row r="437" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C437" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D437" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B438" s="2" t="s">
         <v>122</v>
@@ -8841,12 +8836,12 @@
         <v>32</v>
       </c>
       <c r="D438" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B439" s="2" t="s">
         <v>122</v>
@@ -8855,7 +8850,7 @@
         <v>32</v>
       </c>
       <c r="D439" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H439" s="2" t="s">
         <v>100</v>
@@ -8863,7 +8858,7 @@
     </row>
     <row r="440" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B440" s="2" t="s">
         <v>122</v>
@@ -8872,12 +8867,12 @@
         <v>32</v>
       </c>
       <c r="D440" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B441" s="2" t="s">
         <v>122</v>
@@ -8886,12 +8881,12 @@
         <v>32</v>
       </c>
       <c r="D441" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B442" s="2" t="s">
         <v>122</v>
@@ -8900,37 +8895,37 @@
         <v>32</v>
       </c>
       <c r="D442" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="H442" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C443" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D443" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C444" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D444" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C445" s="1" t="s">
         <v>26</v>
@@ -8939,7 +8934,7 @@
         <v>501</v>
       </c>
       <c r="G445" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] z0bug_odoo old data for mk_test_env
</commit_message>
<xml_diff>
--- a/clodoo/transodoo.xlsx
+++ b/clodoo/transodoo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="722">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -1829,12 +1829,6 @@
   </si>
   <si>
     <t xml:space="preserve">l10n_it_lettera_intento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l10n_it_intrastat_statement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l10n_it_intrastat_statement_plus</t>
   </si>
   <si>
     <t xml:space="preserve">l10n_it_invoices_data_communication_fatturapa</t>
@@ -2382,12 +2376,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y445"/>
+  <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A345" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="V364" activeCellId="0" sqref="V364"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A344" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="P356" activeCellId="0" sqref="P356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7611,8 +7605,11 @@
       <c r="H356" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="V356" s="2" t="s">
-        <v>604</v>
+      <c r="Q356" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="Y356" s="1" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7626,10 +7623,10 @@
         <v>199</v>
       </c>
       <c r="H357" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="Q357" s="1" t="s">
         <v>605</v>
-      </c>
-      <c r="Q357" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="Y357" s="1" t="s">
         <v>199</v>
@@ -7648,9 +7645,6 @@
       <c r="H358" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="Q358" s="1" t="s">
-        <v>607</v>
-      </c>
       <c r="Y358" s="1" t="s">
         <v>199</v>
       </c>
@@ -7666,9 +7660,12 @@
         <v>199</v>
       </c>
       <c r="H359" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="Y359" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="M359" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="V359" s="2" t="s">
         <v>199</v>
       </c>
     </row>
@@ -7682,8 +7679,8 @@
       <c r="D360" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="H360" s="2" t="s">
-        <v>609</v>
+      <c r="J360" s="2" t="s">
+        <v>608</v>
       </c>
       <c r="M360" s="1" t="s">
         <v>199</v>
@@ -7702,10 +7699,10 @@
       <c r="D361" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="J361" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="M361" s="1" t="s">
+      <c r="H361" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q361" s="1" t="s">
         <v>199</v>
       </c>
       <c r="V361" s="2" t="s">
@@ -7723,16 +7720,13 @@
         <v>199</v>
       </c>
       <c r="H362" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="Q362" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="I362" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="V362" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="1" t="s">
         <v>219</v>
       </c>
@@ -7743,28 +7737,25 @@
         <v>199</v>
       </c>
       <c r="H363" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="I363" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="V363" s="2"/>
+      <c r="Y363" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="1" t="s">
-        <v>219</v>
+        <v>172</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>346</v>
+        <v>26</v>
       </c>
       <c r="D364" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H364" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="V364" s="2"/>
-      <c r="Y364" s="1" t="s">
-        <v>199</v>
+        <v>108</v>
+      </c>
+      <c r="G364" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7775,10 +7766,10 @@
         <v>26</v>
       </c>
       <c r="D365" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G365" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7789,32 +7780,29 @@
         <v>26</v>
       </c>
       <c r="D366" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G366" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="1" t="s">
-        <v>172</v>
+        <v>612</v>
       </c>
       <c r="C367" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D367" s="2" t="s">
-        <v>112</v>
+      <c r="F367" s="2" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C368" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F368" s="2" t="s">
-        <v>615</v>
+      <c r="D368" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7825,104 +7813,110 @@
         <v>26</v>
       </c>
       <c r="D369" s="2" t="s">
-        <v>2</v>
+        <v>116</v>
+      </c>
+      <c r="G369" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C370" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D370" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G370" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C371" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D371" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="G371" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C372" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D372" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G372" s="1" t="s">
-        <v>120</v>
+        <v>1</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C373" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D373" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G373" s="1" t="s">
-        <v>1</v>
+        <v>122</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C374" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D374" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="G374" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C375" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D375" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G375" s="1" t="s">
-        <v>124</v>
+        <v>616</v>
+      </c>
+      <c r="F375" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="1" t="s">
         <v>617</v>
       </c>
+      <c r="B376" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="C376" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D376" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="F376" s="2" t="s">
-        <v>1</v>
+      <c r="G376" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B377" s="2" t="s">
         <v>122</v>
@@ -7931,15 +7925,15 @@
         <v>32</v>
       </c>
       <c r="D377" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="G377" s="1" t="s">
         <v>620</v>
-      </c>
-      <c r="G377" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B378" s="2" t="s">
         <v>122</v>
@@ -7950,13 +7944,10 @@
       <c r="D378" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="G378" s="1" t="s">
-        <v>622</v>
-      </c>
     </row>
     <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B379" s="2" t="s">
         <v>122</v>
@@ -7965,12 +7956,15 @@
         <v>32</v>
       </c>
       <c r="D379" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="G379" s="1" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B380" s="2" t="s">
         <v>122</v>
@@ -7981,13 +7975,10 @@
       <c r="D380" s="2" t="s">
         <v>624</v>
       </c>
-      <c r="G380" s="1" t="s">
-        <v>625</v>
-      </c>
     </row>
     <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B381" s="2" t="s">
         <v>122</v>
@@ -7996,12 +7987,12 @@
         <v>32</v>
       </c>
       <c r="D381" s="2" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B382" s="2" t="s">
         <v>122</v>
@@ -8010,12 +8001,15 @@
         <v>32</v>
       </c>
       <c r="D382" s="2" t="s">
-        <v>622</v>
+        <v>625</v>
+      </c>
+      <c r="G382" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B383" s="2" t="s">
         <v>122</v>
@@ -8024,7 +8018,7 @@
         <v>32</v>
       </c>
       <c r="D383" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G383" s="1" t="s">
         <v>143</v>
@@ -8032,7 +8026,7 @@
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B384" s="2" t="s">
         <v>122</v>
@@ -8041,15 +8035,12 @@
         <v>32</v>
       </c>
       <c r="D384" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="G384" s="1" t="s">
-        <v>143</v>
+        <v>627</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="1" t="s">
-        <v>619</v>
+        <v>628</v>
       </c>
       <c r="B385" s="2" t="s">
         <v>122</v>
@@ -8058,12 +8049,12 @@
         <v>32</v>
       </c>
       <c r="D385" s="2" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B386" s="2" t="s">
         <v>122</v>
@@ -8072,12 +8063,15 @@
         <v>32</v>
       </c>
       <c r="D386" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
+      </c>
+      <c r="G386" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B387" s="2" t="s">
         <v>122</v>
@@ -8094,7 +8088,7 @@
     </row>
     <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B388" s="2" t="s">
         <v>122</v>
@@ -8103,40 +8097,37 @@
         <v>32</v>
       </c>
       <c r="D388" s="2" t="s">
-        <v>626</v>
-      </c>
-      <c r="G388" s="1" t="s">
-        <v>143</v>
+        <v>620</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="C389" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D389" s="2" t="s">
         <v>630</v>
-      </c>
-      <c r="B389" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C389" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D389" s="2" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="1" t="s">
         <v>631</v>
       </c>
+      <c r="B390" s="2" t="s">
+        <v>632</v>
+      </c>
       <c r="C390" s="1" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D390" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B391" s="2" t="s">
         <v>634</v>
@@ -8147,129 +8138,132 @@
       <c r="D391" s="2" t="s">
         <v>635</v>
       </c>
+      <c r="E391" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="G391" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B392" s="2" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="C392" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D392" s="2" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="E392" s="1" t="s">
-        <v>638</v>
-      </c>
-      <c r="G392" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B393" s="2" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C393" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D393" s="2" t="s">
-        <v>641</v>
-      </c>
-      <c r="E393" s="1" t="s">
         <v>642</v>
+      </c>
+      <c r="G393" s="1" t="s">
+        <v>643</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="C394" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D394" s="2" t="s">
-        <v>644</v>
-      </c>
-      <c r="G394" s="1" t="s">
-        <v>645</v>
+        <v>635</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B395" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C395" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D395" s="2" t="s">
-        <v>637</v>
+        <v>646</v>
+      </c>
+      <c r="F395" s="2" t="s">
+        <v>647</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="C396" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D396" s="2" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="F396" s="2" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B397" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="C397" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D397" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="F397" s="2" t="s">
         <v>652</v>
+      </c>
+      <c r="H397" s="2" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B398" s="2" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C398" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D398" s="2" t="s">
-        <v>654</v>
-      </c>
-      <c r="H398" s="2" t="s">
         <v>655</v>
+      </c>
+      <c r="F398" s="2" t="s">
+        <v>650</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B399" s="2" t="s">
         <v>656</v>
@@ -8280,150 +8274,144 @@
       <c r="D399" s="2" t="s">
         <v>657</v>
       </c>
-      <c r="F399" s="2" t="s">
-        <v>652</v>
+      <c r="E399" s="1" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B400" s="2" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C400" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D400" s="2" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="E400" s="1" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B401" s="2" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C401" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D401" s="2" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="E401" s="1" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B402" s="2" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C402" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D402" s="2" t="s">
-        <v>665</v>
-      </c>
-      <c r="E402" s="1" t="s">
         <v>666</v>
+      </c>
+      <c r="G402" s="1" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B403" s="2" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C403" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D403" s="2" t="s">
-        <v>668</v>
-      </c>
-      <c r="G403" s="1" t="s">
         <v>669</v>
+      </c>
+      <c r="E403" s="1" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B404" s="2" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C404" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D404" s="2" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="E404" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
+      </c>
+      <c r="H404" s="2" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B405" s="2" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="C405" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D405" s="2" t="s">
-        <v>674</v>
-      </c>
-      <c r="E405" s="1" t="s">
-        <v>675</v>
+        <v>642</v>
+      </c>
+      <c r="F405" s="2" t="s">
+        <v>676</v>
       </c>
       <c r="H405" s="2" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B406" s="2" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="C406" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D406" s="2" t="s">
-        <v>644</v>
-      </c>
-      <c r="F406" s="2" t="s">
-        <v>678</v>
-      </c>
-      <c r="H406" s="2" t="s">
         <v>679</v>
+      </c>
+      <c r="E406" s="1" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="B407" s="2" t="s">
-        <v>680</v>
+        <v>149</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D407" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E407" s="1" t="s">
         <v>681</v>
-      </c>
-      <c r="E407" s="1" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8433,7 +8421,10 @@
       <c r="C408" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E408" s="1" t="s">
+      <c r="D408" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="G408" s="1" t="s">
         <v>683</v>
       </c>
     </row>
@@ -8444,11 +8435,8 @@
       <c r="C409" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D409" s="2" t="s">
+      <c r="E409" s="1" t="s">
         <v>684</v>
-      </c>
-      <c r="G409" s="1" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8459,7 +8447,7 @@
         <v>26</v>
       </c>
       <c r="E410" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8470,7 +8458,7 @@
         <v>26</v>
       </c>
       <c r="E411" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8480,7 +8468,10 @@
       <c r="C412" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E412" s="1" t="s">
+      <c r="D412" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G412" s="1" t="s">
         <v>688</v>
       </c>
     </row>
@@ -8505,11 +8496,8 @@
       <c r="C414" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D414" s="2" t="s">
+      <c r="E414" s="1" t="s">
         <v>691</v>
-      </c>
-      <c r="G414" s="1" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8520,7 +8508,7 @@
         <v>26</v>
       </c>
       <c r="E415" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8531,7 +8519,7 @@
         <v>26</v>
       </c>
       <c r="E416" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8541,7 +8529,10 @@
       <c r="C417" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E417" s="1" t="s">
+      <c r="D417" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="G417" s="1" t="s">
         <v>695</v>
       </c>
     </row>
@@ -8552,11 +8543,8 @@
       <c r="C418" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D418" s="2" t="s">
-        <v>696</v>
-      </c>
-      <c r="G418" s="1" t="s">
-        <v>697</v>
+      <c r="E418" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8567,23 +8555,26 @@
         <v>26</v>
       </c>
       <c r="E419" s="1" t="s">
-        <v>2</v>
+        <v>696</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="1" t="s">
-        <v>149</v>
+        <v>697</v>
       </c>
       <c r="C420" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D420" s="2" t="s">
+        <v>698</v>
+      </c>
       <c r="E420" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="1" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C421" s="1" t="s">
         <v>26</v>
@@ -8597,85 +8588,85 @@
     </row>
     <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="1" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C422" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D422" s="2" t="s">
-        <v>702</v>
-      </c>
       <c r="E422" s="1" t="s">
-        <v>703</v>
+        <v>681</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="1" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C423" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E423" s="1" t="s">
-        <v>683</v>
+        <v>702</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="1" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C424" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D424" s="2" t="s">
+        <v>703</v>
+      </c>
       <c r="E424" s="1" t="s">
         <v>704</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="1" t="s">
-        <v>699</v>
+        <v>705</v>
       </c>
       <c r="C425" s="1" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="D425" s="2" t="s">
-        <v>705</v>
-      </c>
-      <c r="E425" s="1" t="s">
         <v>706</v>
+      </c>
+      <c r="G425" s="1" t="s">
+        <v>707</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="1" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C426" s="1" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="D426" s="2" t="s">
-        <v>708</v>
-      </c>
-      <c r="G426" s="1" t="s">
-        <v>709</v>
+        <v>91</v>
+      </c>
+      <c r="H426" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="1" t="s">
-        <v>707</v>
+        <v>705</v>
+      </c>
+      <c r="B427" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="C427" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D427" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H427" s="2" t="s">
-        <v>92</v>
+        <v>621</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="1" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B428" s="2" t="s">
         <v>122</v>
@@ -8684,12 +8675,12 @@
         <v>32</v>
       </c>
       <c r="D428" s="2" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="1" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B429" s="2" t="s">
         <v>122</v>
@@ -8698,12 +8689,12 @@
         <v>32</v>
       </c>
       <c r="D429" s="2" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="1" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B430" s="2" t="s">
         <v>122</v>
@@ -8712,12 +8703,15 @@
         <v>32</v>
       </c>
       <c r="D430" s="2" t="s">
-        <v>622</v>
+        <v>708</v>
+      </c>
+      <c r="G430" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="1" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B431" s="2" t="s">
         <v>122</v>
@@ -8726,7 +8720,7 @@
         <v>32</v>
       </c>
       <c r="D431" s="2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="G431" s="1" t="s">
         <v>100</v>
@@ -8734,7 +8728,7 @@
     </row>
     <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="1" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B432" s="2" t="s">
         <v>122</v>
@@ -8743,7 +8737,7 @@
         <v>32</v>
       </c>
       <c r="D432" s="2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="G432" s="1" t="s">
         <v>100</v>
@@ -8751,7 +8745,7 @@
     </row>
     <row r="433" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="1" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B433" s="2" t="s">
         <v>122</v>
@@ -8760,15 +8754,12 @@
         <v>32</v>
       </c>
       <c r="D433" s="2" t="s">
-        <v>712</v>
-      </c>
-      <c r="G433" s="1" t="s">
-        <v>100</v>
+        <v>627</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="1" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B434" s="2" t="s">
         <v>122</v>
@@ -8777,12 +8768,15 @@
         <v>32</v>
       </c>
       <c r="D434" s="2" t="s">
-        <v>629</v>
+        <v>711</v>
+      </c>
+      <c r="G434" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="1" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B435" s="2" t="s">
         <v>122</v>
@@ -8791,7 +8785,7 @@
         <v>32</v>
       </c>
       <c r="D435" s="2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="G435" s="1" t="s">
         <v>100</v>
@@ -8799,35 +8793,32 @@
     </row>
     <row r="436" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="B436" s="2" t="s">
-        <v>122</v>
+        <v>713</v>
       </c>
       <c r="C436" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D436" s="2" t="s">
         <v>714</v>
       </c>
-      <c r="G436" s="1" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="437" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="1" t="s">
-        <v>715</v>
+        <v>713</v>
+      </c>
+      <c r="B437" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="C437" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D437" s="2" t="s">
-        <v>716</v>
+        <v>621</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="1" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B438" s="2" t="s">
         <v>122</v>
@@ -8836,12 +8827,15 @@
         <v>32</v>
       </c>
       <c r="D438" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
+      </c>
+      <c r="H438" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="1" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B439" s="2" t="s">
         <v>122</v>
@@ -8852,13 +8846,10 @@
       <c r="D439" s="2" t="s">
         <v>624</v>
       </c>
-      <c r="H439" s="2" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="440" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="1" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B440" s="2" t="s">
         <v>122</v>
@@ -8867,12 +8858,12 @@
         <v>32</v>
       </c>
       <c r="D440" s="2" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="1" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B441" s="2" t="s">
         <v>122</v>
@@ -8881,24 +8872,21 @@
         <v>32</v>
       </c>
       <c r="D441" s="2" t="s">
-        <v>622</v>
+        <v>715</v>
+      </c>
+      <c r="H441" s="2" t="s">
+        <v>620</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="1" t="s">
-        <v>715</v>
-      </c>
-      <c r="B442" s="2" t="s">
-        <v>122</v>
+        <v>716</v>
       </c>
       <c r="C442" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D442" s="2" t="s">
         <v>717</v>
-      </c>
-      <c r="H442" s="2" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8920,23 +8908,13 @@
         <v>26</v>
       </c>
       <c r="D444" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="G444" s="1" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="445" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A445" s="1" t="s">
-        <v>722</v>
-      </c>
-      <c r="C445" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D445" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="G445" s="1" t="s">
-        <v>723</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
[IMP] Stable version, more tests
</commit_message>
<xml_diff>
--- a/clodoo/transodoo.xlsx
+++ b/clodoo/transodoo.xlsx
@@ -2673,10 +2673,10 @@
   </sheetPr>
   <dimension ref="A1:AE1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="630" topLeftCell="N267" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C279" activeCellId="0" sqref="C279"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="630" topLeftCell="N139" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="T161" activeCellId="0" sqref="T161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5391,7 +5391,8 @@
         <v>287</v>
       </c>
       <c r="G161" s="2"/>
-      <c r="H161" s="1" t="s">
+      <c r="H161" s="0"/>
+      <c r="J161" s="1" t="s">
         <v>288</v>
       </c>
     </row>

</xml_diff>